<commit_message>
dev: optimize point sheet status
</commit_message>
<xml_diff>
--- a/test/data/test-modbus-tcp-sheet.xlsx
+++ b/test/data/test-modbus-tcp-sheet.xlsx
@@ -65,10 +65,10 @@
     <t>127.0.0.1:502</t>
   </si>
   <si>
-    <t>FLOAT32</t>
-  </si>
-  <si>
-    <t>DCBA</t>
+    <t>INT16</t>
+  </si>
+  <si>
+    <t>AB</t>
   </si>
   <si>
     <t>a2</t>
@@ -755,7 +755,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -763,6 +763,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1293,7 +1296,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H16"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1357,12 +1360,12 @@
         <v>11</v>
       </c>
       <c r="F2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" s="2">
-        <v>2</v>
-      </c>
-      <c r="H2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="2" t="s">
@@ -1389,12 +1392,12 @@
         <v>11</v>
       </c>
       <c r="F3" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G3" s="2">
-        <v>2</v>
-      </c>
-      <c r="H3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -1421,12 +1424,12 @@
         <v>11</v>
       </c>
       <c r="F4" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G4" s="2">
-        <v>2</v>
-      </c>
-      <c r="H4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -1453,12 +1456,12 @@
         <v>11</v>
       </c>
       <c r="F5" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G5" s="2">
-        <v>2</v>
-      </c>
-      <c r="H5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -1485,12 +1488,12 @@
         <v>11</v>
       </c>
       <c r="F6" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G6" s="2">
-        <v>2</v>
-      </c>
-      <c r="H6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="I6" s="2" t="s">
@@ -1517,12 +1520,12 @@
         <v>11</v>
       </c>
       <c r="F7" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G7" s="2">
-        <v>2</v>
-      </c>
-      <c r="H7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -1549,12 +1552,12 @@
         <v>11</v>
       </c>
       <c r="F8" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G8" s="2">
-        <v>2</v>
-      </c>
-      <c r="H8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="I8" s="2" t="s">
@@ -1581,12 +1584,12 @@
         <v>11</v>
       </c>
       <c r="F9" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G9" s="2">
-        <v>2</v>
-      </c>
-      <c r="H9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="I9" s="2" t="s">
@@ -1613,12 +1616,12 @@
         <v>11</v>
       </c>
       <c r="F10" s="2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G10" s="2">
-        <v>2</v>
-      </c>
-      <c r="H10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="I10" s="2" t="s">
@@ -1645,12 +1648,12 @@
         <v>11</v>
       </c>
       <c r="F11" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G11" s="2">
-        <v>2</v>
-      </c>
-      <c r="H11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="I11" s="2" t="s">
@@ -1677,12 +1680,12 @@
         <v>11</v>
       </c>
       <c r="F12" s="2">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G12" s="2">
-        <v>2</v>
-      </c>
-      <c r="H12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="I12" s="2" t="s">
@@ -1709,12 +1712,12 @@
         <v>11</v>
       </c>
       <c r="F13" s="2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G13" s="2">
-        <v>2</v>
-      </c>
-      <c r="H13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>12</v>
       </c>
       <c r="I13" s="2" t="s">
@@ -1741,12 +1744,12 @@
         <v>11</v>
       </c>
       <c r="F14" s="2">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G14" s="2">
-        <v>2</v>
-      </c>
-      <c r="H14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>12</v>
       </c>
       <c r="I14" s="2" t="s">
@@ -1773,12 +1776,12 @@
         <v>11</v>
       </c>
       <c r="F15" s="2">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G15" s="2">
-        <v>2</v>
-      </c>
-      <c r="H15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>12</v>
       </c>
       <c r="I15" s="2" t="s">
@@ -1805,12 +1808,12 @@
         <v>11</v>
       </c>
       <c r="F16" s="2">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G16" s="2">
-        <v>2</v>
-      </c>
-      <c r="H16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>12</v>
       </c>
       <c r="I16" s="2" t="s">

</xml_diff>